<commit_message>
Section 4: Working with Basic Excel Functions Quiz
</commit_message>
<xml_diff>
--- a/Section 4: Working with Basic Excel Functions/Resources/monthlybudget.xlsx
+++ b/Section 4: Working with Basic Excel Functions/Resources/monthlybudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 4: Working with Basic Excel Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CE0D72-4B70-C744-9DCC-9DB2016E8B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEEA566-4EB4-0D41-97C5-A20F2410743E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{51F0C39A-75DD-F540-B849-5C49F44F8AE5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17260" xr2:uid="{51F0C39A-75DD-F540-B849-5C49F44F8AE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>COUNT</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65875596-FFE2-F64E-A595-6737C2AEB7A0}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +485,7 @@
         <v>3000.55</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F9" si="0">E4/$E$9</f>
+        <f>(E4/$E$9)</f>
         <v>0.58825086260978676</v>
       </c>
     </row>
@@ -500,11 +503,11 @@
         <v>100</v>
       </c>
       <c r="E5">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" ref="E5:E8" si="0">SUM(B5:D5)</f>
         <v>325.25</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F5:F9" si="1">(E5/$E$9)</f>
         <v>6.376450752823086E-2</v>
       </c>
     </row>
@@ -522,11 +525,11 @@
         <v>175</v>
       </c>
       <c r="E6">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>525</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10292503136762861</v>
       </c>
     </row>
@@ -544,11 +547,11 @@
         <v>350</v>
       </c>
       <c r="E7">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>925</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.18134410288582181</v>
       </c>
     </row>
@@ -566,11 +569,11 @@
         <v>125</v>
       </c>
       <c r="E8">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>325</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.3715495608532E-2</v>
       </c>
     </row>
@@ -583,20 +586,16 @@
         <v>1650.8</v>
       </c>
       <c r="C9">
-        <f>SUM(C4:C8)</f>
+        <f t="shared" ref="C9:E9" si="2">SUM(C4:C8)</f>
         <v>1700</v>
       </c>
       <c r="D9">
-        <f>SUM(D4:D8)</f>
+        <f t="shared" si="2"/>
         <v>1750</v>
       </c>
       <c r="E9">
-        <f>SUM(B9:D9)</f>
+        <f t="shared" si="2"/>
         <v>5100.8</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -607,6 +606,18 @@
         <f>MIN(B4:B8)</f>
         <v>100</v>
       </c>
+      <c r="C11">
+        <f>MIN(C4:C8)</f>
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <f>MIN(D4:D8)</f>
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <f>MIN(E4:E8)</f>
+        <v>325</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -616,14 +627,66 @@
         <f>MAX(B4:B8)</f>
         <v>1000.55</v>
       </c>
+      <c r="C12">
+        <f>MAX(C4:C8)</f>
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <f>MAX(D4:D8)</f>
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <f>MAX(E4:E8)</f>
+        <v>3000.55</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <f>AVERAGE(B4:B8)</f>
+        <v>330.15999999999997</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C4:C8)</f>
+        <v>340</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D4:D8)</f>
+        <v>350</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E4:E8)</f>
+        <v>1020.1600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>COUNT(B4:B8)</f>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f>COUNT(C4:C8)</f>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f>COUNT(D4:D8)</f>
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <f>COUNT(E4:E8)</f>
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B10:E15 B9" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>